<commit_message>
fixed make_acados_sim with sim_options; improved calc_cp_max_spline with actual calculation of polynomial; fixed hadling of flags in compileProg; improved generation of EKF; updated acados models with polynomial cx tables; updated acados OCP models; fixed minor problem in DISCON_mex; added generation and simulation of acados MPC via DISCON.dll
</commit_message>
<xml_diff>
--- a/ref_sim/openFAST_config_dyn_inflow.xlsx
+++ b/ref_sim/openFAST_config_dyn_inflow.xlsx
@@ -5,11 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="config" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="DLC_List" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="config" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="DLC_List" sheetId="2" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -29,7 +29,7 @@
     <t xml:space="preserve">MainInput</t>
   </si>
   <si>
-    <t xml:space="preserve">../5MW_Baseline/5MW_Land_DLL_WTurb.fst</t>
+    <t xml:space="preserve">../5MW_Baseline/5MW_Land_DLL_MPC.fst</t>
   </si>
   <si>
     <t xml:space="preserve">ElastoDyn</t>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">./sim_dyn_inflow</t>
+    <t xml:space="preserve">./sim_MPC</t>
   </si>
   <si>
     <t xml:space="preserve">Wind directory</t>
@@ -334,44 +334,48 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -447,15 +451,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -465,12 +575,12 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="3" style="1" width="11.55"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -478,7 +588,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -486,7 +596,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>5</v>
       </c>
@@ -494,7 +604,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -502,7 +612,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
@@ -510,7 +620,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -518,7 +628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
         <v>13</v>
       </c>
@@ -526,10 +636,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="16.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
@@ -537,7 +647,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
@@ -545,7 +655,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
         <v>19</v>
       </c>
@@ -553,7 +663,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
         <v>21</v>
       </c>
@@ -561,7 +671,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
         <v>23</v>
       </c>
@@ -569,7 +679,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
         <v>25</v>
       </c>
@@ -577,7 +687,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
         <v>27</v>
       </c>
@@ -585,7 +695,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="15.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
         <v>29</v>
       </c>
@@ -605,14 +715,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Q2" activeCellId="1" sqref="B6 Q2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -756,8 +866,8 @@
       <c r="O3" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="P3" s="0"/>
-      <c r="Q3" s="0"/>
+      <c r="P3" s="10"/>
+      <c r="Q3" s="10"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">

</xml_diff>

<commit_message>
completely new setup with auto installation
</commit_message>
<xml_diff>
--- a/ref_sim/openFAST_config_dyn_inflow.xlsx
+++ b/ref_sim/openFAST_config_dyn_inflow.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="config" sheetId="1" state="visible" r:id="rId3"/>
@@ -71,7 +71,7 @@
     <t xml:space="preserve">Simulation directory</t>
   </si>
   <si>
-    <t xml:space="preserve">./sim_MPC</t>
+    <t xml:space="preserve">./sim_dyn_inflow</t>
   </si>
   <si>
     <t xml:space="preserve">Wind directory</t>
@@ -564,8 +564,8 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="15.6" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -721,7 +721,7 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q2" activeCellId="0" sqref="Q2"/>
     </sheetView>
   </sheetViews>

</xml_diff>